<commit_message>
Add Deny button in every queue.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-next-possible-queues-rules.xlsx
+++ b/acm/rules/drools-next-possible-queues-rules.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\Documents\ACM3\acm-plugins\acm-default-plugins\acm-case-file-plugin\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CE908E97-697E-4186-B333-B6BCBFCFB241}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="338" tabRatio="997"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="345" tabRatio="997" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B17" authorId="0" shapeId="0">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -41,7 +42,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>RuleSet</t>
   </si>
@@ -175,11 +176,20 @@
   <si>
     <t>$model.setDefaultReturnQueue($param);</t>
   </si>
+  <si>
+    <t>$model.setDefaultDenyQueue($param);</t>
+  </si>
+  <si>
+    <t>Default deny queue</t>
+  </si>
+  <si>
+    <t>Default return queue</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
@@ -440,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -471,9 +481,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -587,7 +594,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1032" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1032" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -630,7 +643,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -673,7 +692,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -716,7 +741,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1043,29 +1074,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="E11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.796875"/>
-    <col min="2" max="2" width="24.265625"/>
-    <col min="3" max="3" width="69.53125"/>
-    <col min="4" max="4" width="70.6640625"/>
-    <col min="5" max="5" width="35.73046875"/>
-    <col min="6" max="6" width="36.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625"/>
-    <col min="8" max="1025" width="8.73046875"/>
+    <col min="1" max="1" width="14.85546875"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="69.5703125"/>
+    <col min="4" max="4" width="70.7109375"/>
+    <col min="5" max="5" width="35.7109375"/>
+    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1074,7 +1105,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -1087,7 +1118,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
@@ -1100,147 +1131,156 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="171" x14ac:dyDescent="0.45">
-      <c r="C10" s="20" t="s">
+    <row r="10" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="C10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="19"/>
-    </row>
-    <row r="12" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G11" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="G12" s="19"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G14" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C16" s="23" t="s">
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+      <c r="G16" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -1257,10 +1297,13 @@
         <v>28</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="16" t="s">
         <v>10</v>
@@ -1277,8 +1320,11 @@
       <c r="F18" s="18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G18" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" s="17"/>
       <c r="D19" s="18"/>
     </row>
@@ -1291,7 +1337,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1299,9 +1345,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1310,7 +1356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1318,9 +1364,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>